<commit_message>
added a note to self
</commit_message>
<xml_diff>
--- a/inSALMO Fish Parameters.xlsx
+++ b/inSALMO Fish Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ted\Desktop\predation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32D16CD-0845-4FBC-82D5-F54611CF324F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7802C4-5687-4DE6-95D7-7E8535381CE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="804" firstSheet="11" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33866,7 +33866,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33877,8 +33877,8 @@
     <col min="4" max="4" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
added script for making X values of factorsasd
</commit_message>
<xml_diff>
--- a/inSALMO Fish Parameters.xlsx
+++ b/inSALMO Fish Parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="21"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -464,7 +464,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10370" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10370" uniqueCount="351">
   <si>
     <t xml:space="preserve">fishSpawnVSuit</t>
   </si>
@@ -1123,7 +1123,7 @@
     <t xml:space="preserve">journal</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
+    <t xml:space="preserve">x</t>
   </si>
   <si>
     <t xml:space="preserve">i_units</t>
@@ -1516,6 +1516,9 @@
   </si>
   <si>
     <t xml:space="preserve">Has Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
   </si>
   <si>
     <t xml:space="preserve">Slope 1</t>
@@ -4513,11 +4516,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="13171119"/>
-        <c:axId val="2744352"/>
+        <c:axId val="65277034"/>
+        <c:axId val="9013928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="13171119"/>
+        <c:axId val="65277034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4583,12 +4586,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2744352"/>
+        <c:crossAx val="9013928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2744352"/>
+        <c:axId val="9013928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -4656,7 +4659,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13171119"/>
+        <c:crossAx val="65277034"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4836,11 +4839,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="95036965"/>
-        <c:axId val="81065277"/>
+        <c:axId val="22411727"/>
+        <c:axId val="53281294"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95036965"/>
+        <c:axId val="22411727"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -4883,12 +4886,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81065277"/>
+        <c:crossAx val="53281294"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81065277"/>
+        <c:axId val="53281294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4931,7 +4934,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95036965"/>
+        <c:crossAx val="22411727"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5154,11 +5157,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44326132"/>
-        <c:axId val="70476466"/>
+        <c:axId val="15582447"/>
+        <c:axId val="45838211"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44326132"/>
+        <c:axId val="15582447"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5234,12 +5237,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70476466"/>
+        <c:crossAx val="45838211"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70476466"/>
+        <c:axId val="45838211"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="6"/>
@@ -5316,7 +5319,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44326132"/>
+        <c:crossAx val="15582447"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5466,11 +5469,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="77683736"/>
-        <c:axId val="95053112"/>
+        <c:axId val="18757675"/>
+        <c:axId val="48248240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77683736"/>
+        <c:axId val="18757675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -5513,12 +5516,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95053112"/>
+        <c:crossAx val="48248240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95053112"/>
+        <c:axId val="48248240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5561,7 +5564,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77683736"/>
+        <c:crossAx val="18757675"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5598,9 +5601,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>22320</xdr:colOff>
+      <xdr:colOff>21960</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>136440</xdr:rowOff>
+      <xdr:rowOff>136080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5614,7 +5617,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11459160" y="119160"/>
-          <a:ext cx="6303600" cy="5541480"/>
+          <a:ext cx="6303240" cy="5541120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5642,9 +5645,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>786600</xdr:colOff>
+      <xdr:colOff>786240</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5653,7 +5656,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10445040" y="0"/>
-        <a:ext cx="6293880" cy="5333040"/>
+        <a:ext cx="6293520" cy="5332680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5677,9 +5680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>87480</xdr:colOff>
+      <xdr:colOff>87120</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5692,8 +5695,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7663320" y="474840"/>
-          <a:ext cx="6675840" cy="5327640"/>
+          <a:off x="7662240" y="474840"/>
+          <a:ext cx="6675480" cy="5327280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5714,9 +5717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>75600</xdr:colOff>
+      <xdr:colOff>75240</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5724,8 +5727,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8373960" y="397440"/>
-        <a:ext cx="5166720" cy="4921200"/>
+        <a:off x="8372520" y="397440"/>
+        <a:ext cx="5166360" cy="4920840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5744,9 +5747,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>544320</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
+      <xdr:rowOff>102600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5759,8 +5762,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7569000" y="6114960"/>
-          <a:ext cx="6440760" cy="5227200"/>
+          <a:off x="7567920" y="6114960"/>
+          <a:ext cx="6440040" cy="5226840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5786,9 +5789,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>403200</xdr:colOff>
+      <xdr:colOff>402840</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5797,7 +5800,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="11446920" y="38160"/>
-        <a:ext cx="5811480" cy="2856600"/>
+        <a:ext cx="5811120" cy="2856240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5821,9 +5824,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>537480</xdr:colOff>
+      <xdr:colOff>537120</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5836,8 +5839,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7115760" y="99720"/>
-          <a:ext cx="5923440" cy="4881600"/>
+          <a:off x="7113600" y="99720"/>
+          <a:ext cx="5923440" cy="4881240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5858,9 +5861,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
+      <xdr:colOff>101880</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>157680</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5868,8 +5871,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7748640" y="241200"/>
-        <a:ext cx="4068360" cy="4297680"/>
+        <a:off x="7746480" y="241200"/>
+        <a:ext cx="4068360" cy="4297320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5890,7 +5893,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="1" sqref="J2:J42 D5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6112,7 +6115,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="1" sqref="J2:J42 P8"/>
+      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6249,7 +6252,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M10" activeCellId="1" sqref="J2:J42 M10"/>
+      <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6404,7 +6407,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="J2:J42 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6775,7 +6778,7 @@
   <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G43" activeCellId="1" sqref="J2:J42 G43"/>
+      <selection pane="topLeft" activeCell="G43" activeCellId="0" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8967,7 +8970,7 @@
   <dimension ref="A1:L152"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q19" activeCellId="1" sqref="J2:J42 Q19"/>
+      <selection pane="topLeft" activeCell="Q19" activeCellId="0" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14720,7 +14723,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L25" activeCellId="1" sqref="J2:J42 L25"/>
+      <selection pane="topLeft" activeCell="L25" activeCellId="0" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15207,7 +15210,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F62" activeCellId="1" sqref="J2:J42 F62"/>
+      <selection pane="topLeft" activeCell="F62" activeCellId="0" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15951,7 +15954,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H120" activeCellId="1" sqref="J2:J42 H120"/>
+      <selection pane="bottomLeft" activeCell="H120" activeCellId="0" sqref="H120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20587,7 +20590,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="1" sqref="J2:J42 N17"/>
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21321,7 +21324,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P13" activeCellId="1" sqref="J2:J42 P13"/>
+      <selection pane="topLeft" activeCell="P13" activeCellId="0" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22021,7 +22024,7 @@
   <dimension ref="A1:I204"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J2:J42 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27972,7 +27975,7 @@
   <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J39" activeCellId="0" sqref="J2:J42"/>
+      <selection pane="topLeft" activeCell="J39" activeCellId="0" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31438,8 +31441,8 @@
   </sheetPr>
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="1" sqref="J2:J42 L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -32663,8 +32666,8 @@
   </sheetPr>
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:J42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -34930,7 +34933,7 @@
   <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="1" sqref="J2:J42 A20"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38978,7 +38981,7 @@
   <dimension ref="A1:X51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="1" sqref="J2:J42 A18"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -42683,7 +42686,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M26" activeCellId="1" sqref="J2:J42 M26"/>
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43636,7 +43639,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L34" activeCellId="1" sqref="J2:J42 L34"/>
+      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -44196,7 +44199,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U7" activeCellId="1" sqref="J2:J42 U7"/>
+      <selection pane="topLeft" activeCell="U7" activeCellId="0" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -44701,7 +44704,7 @@
   <dimension ref="A1:L328"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="1" sqref="J2:J42 K1"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -55890,7 +55893,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J2:J42"/>
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -57065,7 +57068,7 @@
   <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J2:J42"/>
+      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -59943,7 +59946,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z5" activeCellId="1" sqref="J2:J42 Z5"/>
+      <selection pane="topLeft" activeCell="Z5" activeCellId="0" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -59990,7 +59993,7 @@
         <v>332</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>219</v>
+        <v>348</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>262</v>
@@ -60213,7 +60216,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="J2:J42 D25"/>
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -60492,7 +60495,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O15" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="P15" s="4" t="n">
         <v>0.0144</v>
@@ -60500,7 +60503,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="O16" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="P16" s="4" t="n">
         <v>0.0186</v>
@@ -60536,7 +60539,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J2:J42"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -60584,7 +60587,7 @@
         <v>332</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>219</v>
+        <v>348</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>262</v>
@@ -60851,7 +60854,7 @@
   <dimension ref="A1:K144"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="J2:J42 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -65824,7 +65827,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="J2:J42 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -65885,7 +65888,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L14" activeCellId="1" sqref="J2:J42 L14"/>
+      <selection pane="bottomLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -66231,7 +66234,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G4" activeCellId="1" sqref="J2:J42 G4"/>
+      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -66445,7 +66448,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J18" activeCellId="0" sqref="J2:J42"/>
+      <selection pane="bottomLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -75601,7 +75604,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="1" sqref="J2:J42 F14"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>